<commit_message>
Formatted some column titles and widths.
</commit_message>
<xml_diff>
--- a/US Housing Monthly Revenue.xlsx
+++ b/US Housing Monthly Revenue.xlsx
@@ -25,7 +25,7 @@
     <t>Avg. Revenue</t>
   </si>
   <si>
-    <t>Periods of Expansion</t>
+    <t># of Expansions</t>
   </si>
   <si>
     <t>Peak</t>
@@ -37,7 +37,7 @@
     <t>Valley</t>
   </si>
   <si>
-    <t>Periods of Recession</t>
+    <t># of Recessions</t>
   </si>
   <si>
     <t>Period</t>
@@ -2324,7 +2324,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="1" max="9" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">

</xml_diff>